<commit_message>
EBEGU-405/782 * Fixing ExcelMerger NamedRange bug * Cleaning up
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/GesuchStichtag.xlsx
+++ b/ebegu-server/src/main/resources/reporting/GesuchStichtag.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\medu\IdeaProjects\ebegu\ebegu-server\src\main\resources\vorlagen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\medu\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </definedNames>
   <calcPr calcId="171027"/>
   <pivotCaches>
-    <pivotCache cacheId="6" r:id="rId3"/>
+    <pivotCache cacheId="8" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>Institution</t>
   </si>
@@ -94,18 +94,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -128,18 +120,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Heading 4" xfId="1" builtinId="19"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -156,7 +145,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Duncan Menzies" refreshedDate="42769.48698530093" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="1">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Duncan Menzies" refreshedDate="42773.561076620368" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="1">
   <cacheSource type="worksheet">
     <worksheetSource name="GesuchStichtagPivottableData"/>
   </cacheSource>
@@ -214,8 +203,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
-  <location ref="B4:G7" firstHeaderRow="0" firstDataRow="1" firstDataCol="3" rowPageCount="1" colPageCount="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+  <location ref="B4:G6" firstHeaderRow="0" firstDataRow="1" firstDataCol="3" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" compact="0" showAll="0" defaultSubtotal="0">
       <items count="1">
@@ -229,7 +218,7 @@
     </pivotField>
     <pivotField axis="axisRow" compact="0" showAll="0" defaultSubtotal="0">
       <items count="1">
-        <item x="0"/>
+        <item sd="0" x="0"/>
       </items>
     </pivotField>
     <pivotField axis="axisPage" compact="0" showAll="0" defaultSubtotal="0">
@@ -246,14 +235,11 @@
     <field x="2"/>
     <field x="0"/>
   </rowFields>
-  <rowItems count="3">
+  <rowItems count="2">
     <i>
       <x/>
     </i>
     <i r="1">
-      <x/>
-    </i>
-    <i r="2">
       <x/>
     </i>
   </rowItems>
@@ -585,17 +571,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G7"/>
+  <dimension ref="B2:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:D6"/>
-      <pivotSelection pane="bottomRight" showHeader="1" dimension="1" activeRow="6" activeCol="2" click="1" r:id="rId1">
-        <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-          <references count="1">
-            <reference field="2" count="0"/>
-          </references>
-        </pivotArea>
-      </pivotSelection>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -668,21 +647,13 @@
       <c r="C6" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="2">
+      <c r="E6" s="2">
         <v>0</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F6" s="2">
         <v>0</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G6" s="2">
         <v>0</v>
       </c>
     </row>
@@ -695,8 +666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -711,25 +682,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
EBEGU-405/782 *code cleanup *adding Report test dataset *formatting and cosmetic changes to report templates
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/GesuchStichtag.xlsx
+++ b/ebegu-server/src/main/resources/reporting/GesuchStichtag.xlsx
@@ -20,7 +20,7 @@
   </definedNames>
   <calcPr calcId="171027"/>
   <pivotCaches>
-    <pivotCache cacheId="8" r:id="rId3"/>
+    <pivotCache cacheId="11" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>Institution</t>
   </si>
@@ -57,15 +57,6 @@
     <t>(All)</t>
   </si>
   <si>
-    <t>Sum of NichtFreigegeben</t>
-  </si>
-  <si>
-    <t>Sum of Mahnungen</t>
-  </si>
-  <si>
-    <t>Sum of Beschwerde</t>
-  </si>
-  <si>
     <t>{bgNummer}</t>
   </si>
   <si>
@@ -88,13 +79,22 @@
   </si>
   <si>
     <t>{repeatGesuchStichtagRow}</t>
+  </si>
+  <si>
+    <t>Offene Mahnungen</t>
+  </si>
+  <si>
+    <t>Nicht freigegebene Gesuche</t>
+  </si>
+  <si>
+    <t>Offene Beschwerden</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,16 +102,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -119,19 +133,321 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" pivotButton="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="28">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <family val="2"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <family val="2"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <family val="2"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <family val="2"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <family val="2"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <family val="2"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <family val="2"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <family val="2"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <family val="2"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <family val="2"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <family val="2"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <family val="2"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <family val="2"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <family val="2"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <family val="2"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <family val="2"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <family val="2"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <family val="2"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -145,15 +461,13 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Duncan Menzies" refreshedDate="42773.561076620368" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="1">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Duncan Menzies" refreshedDate="42776.611577083335" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="1">
   <cacheSource type="worksheet">
     <worksheetSource name="GesuchStichtagPivottableData"/>
   </cacheSource>
   <cacheFields count="7">
     <cacheField name="BGNummer" numFmtId="0">
-      <sharedItems count="1">
-        <s v="{bgNummer}"/>
-      </sharedItems>
+      <sharedItems/>
     </cacheField>
     <cacheField name="Institution" numFmtId="0">
       <sharedItems count="1">
@@ -191,7 +505,7 @@
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="1">
   <r>
-    <x v="0"/>
+    <s v="{bgNummer}"/>
     <x v="0"/>
     <x v="0"/>
     <x v="0"/>
@@ -203,14 +517,10 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
-  <location ref="B4:G6" firstHeaderRow="0" firstDataRow="1" firstDataCol="3" rowPageCount="1" colPageCount="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+  <location ref="B4:F6" firstHeaderRow="0" firstDataRow="1" firstDataCol="2" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="7">
-    <pivotField axis="axisRow" compact="0" showAll="0" defaultSubtotal="0">
-      <items count="1">
-        <item x="0"/>
-      </items>
-    </pivotField>
+    <pivotField compact="0" showAll="0" defaultSubtotal="0"/>
     <pivotField axis="axisRow" compact="0" showAll="0" defaultSubtotal="0">
       <items count="1">
         <item x="0"/>
@@ -230,10 +540,9 @@
     <pivotField dataField="1" compact="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dataField="1" compact="0" showAll="0" defaultSubtotal="0"/>
   </pivotFields>
-  <rowFields count="3">
+  <rowFields count="2">
     <field x="1"/>
     <field x="2"/>
-    <field x="0"/>
   </rowFields>
   <rowItems count="2">
     <i>
@@ -261,11 +570,175 @@
     <pageField fld="3" hier="-1"/>
   </pageFields>
   <dataFields count="3">
-    <dataField name="Sum of NichtFreigegeben" fld="4" baseField="0" baseItem="0"/>
-    <dataField name="Sum of Mahnungen" fld="5" baseField="0" baseItem="0"/>
-    <dataField name="Sum of Beschwerde" fld="6" baseField="0" baseItem="0"/>
+    <dataField name="Nicht freigegebene Gesuche" fld="4" baseField="1" baseItem="0"/>
+    <dataField name="Offene Mahnungen" fld="5" baseField="0" baseItem="0"/>
+    <dataField name="Offene Beschwerden" fld="6" baseField="0" baseItem="0"/>
   </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <formats count="28">
+    <format dxfId="27">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="26">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="25">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="24">
+      <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
+    </format>
+    <format dxfId="23">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="22">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="1" count="0" selected="0"/>
+          <reference field="2" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="21">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="3">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="20">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="19">
+      <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
+    </format>
+    <format dxfId="18">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="3">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="17">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="16">
+      <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
+    </format>
+    <format dxfId="15">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="3">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="14">
+      <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisPage" fieldPosition="0"/>
+    </format>
+    <format dxfId="13">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="12">
+      <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
+    </format>
+    <format dxfId="11">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="10">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="1" count="0" selected="0"/>
+          <reference field="2" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="9">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="8">
+      <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
+    </format>
+    <format dxfId="7">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="6">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="1" count="0" selected="0"/>
+          <reference field="2" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="5">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="4">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="1" count="0" selected="0"/>
+          <reference field="2" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="3">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="2">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="1" count="0" selected="0"/>
+          <reference field="2" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="1">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="1" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="0">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="1" count="0" selected="0"/>
+          <reference field="2" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
@@ -571,18 +1044,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G6"/>
+  <dimension ref="B2:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="21.5" customWidth="1"/>
-    <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="20.75" customWidth="1"/>
-    <col min="6" max="6" width="16.125" customWidth="1"/>
+    <col min="2" max="2" width="21.5" customWidth="1"/>
+    <col min="3" max="3" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.25" customWidth="1"/>
     <col min="8" max="8" width="30.125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="27.75" bestFit="1" customWidth="1"/>
@@ -607,53 +1081,52 @@
     <col min="28" max="28" width="35.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="D4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
-        <v>13</v>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="5"/>
+      <c r="C6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
       </c>
       <c r="E6" s="2">
         <v>0</v>
       </c>
       <c r="F6" s="2">
-        <v>0</v>
-      </c>
-      <c r="G6" s="2">
         <v>0</v>
       </c>
     </row>
@@ -706,28 +1179,28 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>15</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EBEGU-937: Mutationsflags für Betreuung, Abwesenheit und Kind in Statistik Gesuch (Zeitraum) einbauen
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/GesuchStichtag.xlsx
+++ b/ebegu-server/src/main/resources/reporting/GesuchStichtag.xlsx
@@ -1,29 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\medu\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4506"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="GesuchStichtagPivottableData">Data!$A$1:$G$2</definedName>
+    <definedName name="GesuchStichtagPivottableData">Data!$A$1:$H$2</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="125725"/>
   <pivotCaches>
-    <pivotCache cacheId="11" r:id="rId3"/>
+    <pivotCache cacheId="5" r:id="rId3"/>
   </pivotCaches>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -31,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>Institution</t>
   </si>
@@ -54,9 +49,6 @@
     <t>BGNummer</t>
   </si>
   <si>
-    <t>(All)</t>
-  </si>
-  <si>
     <t>{bgNummer}</t>
   </si>
   <si>
@@ -88,13 +80,25 @@
   </si>
   <si>
     <t>Offene Beschwerden</t>
+  </si>
+  <si>
+    <t>Values</t>
+  </si>
+  <si>
+    <t>(Alle)</t>
+  </si>
+  <si>
+    <t>{gesuchId}</t>
+  </si>
+  <si>
+    <t>Gesuch LaufNr</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,124 +156,372 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" pivotButton="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" pivotButton="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <family val="2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <family val="2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <family val="2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <family val="2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <family val="2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <family val="2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <family val="2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <family val="2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <family val="2"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <family val="2"/>
+  <dxfs count="56">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
       </font>
     </dxf>
     <dxf>
@@ -461,11 +713,11 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Duncan Menzies" refreshedDate="42776.611577083335" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="1">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Franziska Herger" refreshedDate="42804.539470949072" createdVersion="6" refreshedVersion="3" minRefreshableVersion="3" recordCount="1">
   <cacheSource type="worksheet">
     <worksheetSource name="GesuchStichtagPivottableData"/>
   </cacheSource>
-  <cacheFields count="7">
+  <cacheFields count="8">
     <cacheField name="BGNummer" numFmtId="0">
       <sharedItems/>
     </cacheField>
@@ -483,6 +735,9 @@
       <sharedItems count="1">
         <s v="{periode}"/>
       </sharedItems>
+    </cacheField>
+    <cacheField name="GesuchId" numFmtId="0">
+      <sharedItems/>
     </cacheField>
     <cacheField name="NichtFreigegeben" numFmtId="0">
       <sharedItems/>
@@ -509,6 +764,7 @@
     <x v="0"/>
     <x v="0"/>
     <x v="0"/>
+    <s v="{gesuchId}"/>
     <s v="{nichtFreigegeben}"/>
     <s v="{mahnungen}"/>
     <s v="{beschwerde}"/>
@@ -517,9 +773,9 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
-  <location ref="B4:F6" firstHeaderRow="0" firstDataRow="1" firstDataCol="2" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="7">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="3" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+  <location ref="B4:F7" firstHeaderRow="1" firstDataRow="2" firstDataCol="2" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="8">
     <pivotField compact="0" showAll="0" defaultSubtotal="0"/>
     <pivotField axis="axisRow" compact="0" showAll="0" defaultSubtotal="0">
       <items count="1">
@@ -536,6 +792,7 @@
         <item x="0"/>
       </items>
     </pivotField>
+    <pivotField compact="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dataField="1" compact="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dataField="1" compact="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dataField="1" compact="0" showAll="0" defaultSubtotal="0"/>
@@ -570,31 +827,31 @@
     <pageField fld="3" hier="-1"/>
   </pageFields>
   <dataFields count="3">
-    <dataField name="Nicht freigegebene Gesuche" fld="4" baseField="1" baseItem="0"/>
-    <dataField name="Offene Mahnungen" fld="5" baseField="0" baseItem="0"/>
-    <dataField name="Offene Beschwerden" fld="6" baseField="0" baseItem="0"/>
+    <dataField name="Nicht freigegebene Gesuche" fld="5" baseField="1" baseItem="0"/>
+    <dataField name="Offene Mahnungen" fld="6" baseField="0" baseItem="0"/>
+    <dataField name="Offene Beschwerden" fld="7" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="28">
-    <format dxfId="27">
+    <format dxfId="55">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="26">
+    <format dxfId="54">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="25">
+    <format dxfId="53">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="24">
+    <format dxfId="52">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="23">
+    <format dxfId="51">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="22">
+    <format dxfId="50">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="0" selected="0"/>
@@ -602,7 +859,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="21">
+    <format dxfId="49">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="3">
@@ -613,13 +870,13 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="20">
+    <format dxfId="48">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="19">
+    <format dxfId="47">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="18">
+    <format dxfId="46">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="3">
@@ -630,13 +887,13 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="17">
+    <format dxfId="45">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="16">
+    <format dxfId="44">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="15">
+    <format dxfId="43">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="3">
@@ -647,23 +904,23 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="14">
+    <format dxfId="42">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisPage" fieldPosition="0"/>
     </format>
-    <format dxfId="13">
+    <format dxfId="41">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="12">
+    <format dxfId="40">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="11">
+    <format dxfId="39">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="10">
+    <format dxfId="38">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="0" selected="0"/>
@@ -671,20 +928,20 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="9">
+    <format dxfId="37">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="8">
+    <format dxfId="36">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="7">
+    <format dxfId="35">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="6">
+    <format dxfId="34">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="0" selected="0"/>
@@ -692,14 +949,14 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="5">
+    <format dxfId="33">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="4">
+    <format dxfId="32">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="0" selected="0"/>
@@ -707,14 +964,14 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="3">
+    <format dxfId="31">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="2">
+    <format dxfId="30">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="0" selected="0"/>
@@ -722,14 +979,14 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="1">
+    <format dxfId="29">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="0">
+    <format dxfId="28">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="0" selected="0"/>
@@ -790,7 +1047,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -842,7 +1099,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1036,97 +1293,106 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="21.5" customWidth="1"/>
-    <col min="3" max="3" width="14.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.25" customWidth="1"/>
-    <col min="8" max="8" width="30.125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.75" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.75" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="31.625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="34.25" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="35.375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="26.375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="32.375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="24.625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="24.875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="27.875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="21.625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="21.75" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="23.375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="29.25" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="36.375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="33.375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="40.125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="35.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" customWidth="1"/>
+    <col min="8" max="8" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="35.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6">
       <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
+    <row r="4" spans="2:6">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="2:6">
+      <c r="B5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>18</v>
-      </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
+    <row r="6" spans="2:6">
+      <c r="B6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="2:6">
+      <c r="B7" s="5"/>
+      <c r="C7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="5"/>
-      <c r="C6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="2">
+      <c r="D7" s="2">
         <v>0</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E7" s="2">
         <v>0</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F7" s="2">
         <v>0</v>
       </c>
     </row>
@@ -1136,25 +1402,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.625" customWidth="1"/>
-    <col min="2" max="2" width="29.25" customWidth="1"/>
-    <col min="3" max="3" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.875" customWidth="1"/>
-    <col min="5" max="5" width="17.625" customWidth="1"/>
-    <col min="6" max="6" width="12.125" customWidth="1"/>
-    <col min="7" max="7" width="16.125" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="29.28515625" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1168,39 +1435,45 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EBEGU-937 * renaming report column gesuchID to gesuchLaufNr to maintain naming consistency
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/GesuchStichtag.xlsx
+++ b/ebegu-server/src/main/resources/reporting/GesuchStichtag.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4506"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\medu\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" activeTab="1"/>
   </bookViews>
@@ -17,8 +22,8 @@
   <pivotCaches>
     <pivotCache cacheId="5" r:id="rId3"/>
   </pivotCaches>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -85,20 +90,20 @@
     <t>Values</t>
   </si>
   <si>
-    <t>(Alle)</t>
-  </si>
-  <si>
-    <t>{gesuchId}</t>
-  </si>
-  <si>
-    <t>Gesuch LaufNr</t>
+    <t>(All)</t>
+  </si>
+  <si>
+    <t>GesuchLaufNr</t>
+  </si>
+  <si>
+    <t>{gesuchLaufNr}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -166,7 +171,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" pivotButton="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="56">
     <dxf>
@@ -713,7 +718,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Franziska Herger" refreshedDate="42804.539470949072" createdVersion="6" refreshedVersion="3" minRefreshableVersion="3" recordCount="1">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Duncan Menzies" refreshedDate="42808.580553472224" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="1">
   <cacheSource type="worksheet">
     <worksheetSource name="GesuchStichtagPivottableData"/>
   </cacheSource>
@@ -736,7 +741,7 @@
         <s v="{periode}"/>
       </sharedItems>
     </cacheField>
-    <cacheField name="GesuchId" numFmtId="0">
+    <cacheField name="GesuchLaufNr" numFmtId="0">
       <sharedItems/>
     </cacheField>
     <cacheField name="NichtFreigegeben" numFmtId="0">
@@ -773,7 +778,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="3" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
   <location ref="B4:F7" firstHeaderRow="1" firstDataRow="2" firstDataCol="2" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="8">
     <pivotField compact="0" showAll="0" defaultSubtotal="0"/>
@@ -792,7 +797,7 @@
         <item x="0"/>
       </items>
     </pivotField>
-    <pivotField compact="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField compact="0" showAll="0"/>
     <pivotField dataField="1" compact="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dataField="1" compact="0" showAll="0" defaultSubtotal="0"/>
     <pivotField dataField="1" compact="0" showAll="0" defaultSubtotal="0"/>
@@ -997,8 +1002,8 @@
   </formats>
   <pivotTableStyleInfo showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
     </ext>
   </extLst>
 </pivotTableDefinition>
@@ -1047,7 +1052,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1099,7 +1104,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1293,52 +1298,52 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" customWidth="1"/>
-    <col min="8" max="8" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="36.42578125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="40.140625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.375" customWidth="1"/>
+    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.25" customWidth="1"/>
+    <col min="8" max="8" width="30.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.75" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.75" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="31.625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="34.25" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="35.375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="32.375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="30.375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="24.625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="24.875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="27.875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="21.625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="21.75" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23.375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="29.25" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="36.375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="33.375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="40.125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="35.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
@@ -1346,7 +1351,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="2:6">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="6" t="s">
@@ -1355,7 +1360,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="2:6">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>0</v>
       </c>
@@ -1372,7 +1377,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="2:6">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>8</v>
       </c>
@@ -1381,7 +1386,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="2:6">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="5"/>
       <c r="C7" s="5" t="s">
         <v>9</v>
@@ -1402,26 +1407,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" customWidth="1"/>
-    <col min="2" max="2" width="29.28515625" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" customWidth="1"/>
-    <col min="8" max="8" width="16.140625" customWidth="1"/>
+    <col min="1" max="1" width="13.625" customWidth="1"/>
+    <col min="2" max="2" width="29.25" customWidth="1"/>
+    <col min="3" max="3" width="21.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.875" customWidth="1"/>
+    <col min="5" max="5" width="13.625" customWidth="1"/>
+    <col min="6" max="6" width="17.625" customWidth="1"/>
+    <col min="7" max="7" width="12.125" customWidth="1"/>
+    <col min="8" max="8" width="16.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1435,7 +1440,7 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
@@ -1447,7 +1452,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1461,7 +1466,7 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
EBEGU-1151: Statistik: Gesuchsteller nach Zeitraum - Spalten fehlen: Spalten eingefügt, bei den Gesuchsreports die Daten-Tabs ausgeblendet, Fokus auf A1
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/GesuchStichtag.xlsx
+++ b/ebegu-server/src/main/resources/reporting/GesuchStichtag.xlsx
@@ -1,19 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\medu\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
-    <sheet name="Data" sheetId="2" r:id="rId2"/>
+    <sheet name="Data" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="GesuchStichtagPivottableData">Data!$A$1:$H$2</definedName>
@@ -22,8 +17,8 @@
   <pivotCaches>
     <pivotCache cacheId="5" r:id="rId3"/>
   </pivotCaches>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -90,20 +85,20 @@
     <t>Values</t>
   </si>
   <si>
-    <t>(All)</t>
-  </si>
-  <si>
     <t>GesuchLaufNr</t>
   </si>
   <si>
     <t>{gesuchLaufNr}</t>
+  </si>
+  <si>
+    <t>(Alle)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -171,7 +166,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" pivotButton="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="56">
     <dxf>
@@ -718,7 +713,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Duncan Menzies" refreshedDate="42808.580553472224" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="1">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Franziska Herger" refreshedDate="42920.534361458333" createdVersion="6" refreshedVersion="3" minRefreshableVersion="3" recordCount="1">
   <cacheSource type="worksheet">
     <worksheetSource name="GesuchStichtagPivottableData"/>
   </cacheSource>
@@ -769,7 +764,7 @@
     <x v="0"/>
     <x v="0"/>
     <x v="0"/>
-    <s v="{gesuchId}"/>
+    <s v="{gesuchLaufNr}"/>
     <s v="{nichtFreigegeben}"/>
     <s v="{mahnungen}"/>
     <s v="{beschwerde}"/>
@@ -778,7 +773,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="3" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
   <location ref="B4:F7" firstHeaderRow="1" firstDataRow="2" firstDataCol="2" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="8">
     <pivotField compact="0" showAll="0" defaultSubtotal="0"/>
@@ -1052,7 +1047,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1104,7 +1099,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1298,60 +1293,58 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="21.375" customWidth="1"/>
-    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.25" customWidth="1"/>
-    <col min="8" max="8" width="30.125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.75" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.75" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="31.625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="34.25" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="35.375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="26.375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="32.375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="30.375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="24.625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="24.875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="27.875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="21.625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="21.75" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="23.375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="29.25" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="36.375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="33.375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="40.125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="35.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" customWidth="1"/>
+    <col min="8" max="8" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="35.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6">
       <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="6" t="s">
@@ -1360,7 +1353,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6">
       <c r="B5" s="3" t="s">
         <v>0</v>
       </c>
@@ -1377,7 +1370,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6">
       <c r="B6" s="5" t="s">
         <v>8</v>
       </c>
@@ -1386,7 +1379,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6">
       <c r="B7" s="5"/>
       <c r="C7" s="5" t="s">
         <v>9</v>
@@ -1407,26 +1400,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.625" customWidth="1"/>
-    <col min="2" max="2" width="29.25" customWidth="1"/>
-    <col min="3" max="3" width="21.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.875" customWidth="1"/>
-    <col min="5" max="5" width="13.625" customWidth="1"/>
-    <col min="6" max="6" width="17.625" customWidth="1"/>
-    <col min="7" max="7" width="12.125" customWidth="1"/>
-    <col min="8" max="8" width="16.125" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="29.28515625" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1440,7 +1433,7 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
@@ -1452,7 +1445,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1466,7 +1459,7 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
EBEGU-1351: Bei allen Statistiken das "Data"-Tab wieder einblenden
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/GesuchStichtag.xlsx
+++ b/ebegu-server/src/main/resources/reporting/GesuchStichtag.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
-    <sheet name="Data" sheetId="2" state="hidden" r:id="rId2"/>
+    <sheet name="Data" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="GesuchStichtagPivottableData">Data!$A$1:$H$2</definedName>
@@ -713,7 +713,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Franziska Herger" refreshedDate="42920.534361458333" createdVersion="6" refreshedVersion="3" minRefreshableVersion="3" recordCount="1">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Franziska Herger" refreshedDate="42992.666940277777" createdVersion="6" refreshedVersion="3" minRefreshableVersion="3" recordCount="1">
   <cacheSource type="worksheet">
     <worksheetSource name="GesuchStichtagPivottableData"/>
   </cacheSource>
@@ -1293,7 +1293,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1303,7 +1303,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
@@ -1403,8 +1403,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>

</xml_diff>